<commit_message>
Performance testing Release 1.3.x v0.4
Signed-off-by: Deepesh Gurung <deepesh.gurung@technoforte.co.in>
</commit_message>
<xml_diff>
--- a/performance-test/packet-credential-processing/MOSIP_TPS_Thread_setting_calculator-packet_credential_processing.xlsx
+++ b/performance-test/packet-credential-processing/MOSIP_TPS_Thread_setting_calculator-packet_credential_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PerfScripts\Release\Platform1.3.x\performance-test\packet-credential-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718FB06F-AD50-40DD-90E4-7EAD5D5304C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72FE6F6-6565-4169-BEFF-2580A7E8E909}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00F0FE37-4E08-4BBA-8E9E-0C9A5473C445}"/>
   </bookViews>
@@ -109,10 +109,6 @@
     <t>From Test Execution</t>
   </si>
   <si>
-    <t>Constant Throughput Limit
-(per minute)</t>
-  </si>
-  <si>
     <t>Totals --&gt;</t>
   </si>
   <si>
@@ -161,6 +157,10 @@
     <t>Scenario Reponse Time
 (From shakeout test)
  (ms) (Average)</t>
+  </si>
+  <si>
+    <t>Constant Throughput Timer
+(Samples per minute)</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -810,12 +810,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -941,6 +935,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1264,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EF0A02-FD69-493C-AB91-7265D86F2CBF}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,26 +1287,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="H1" s="60" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="A1" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="H1" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="50">
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="48">
         <v>100</v>
       </c>
       <c r="E2" s="2"/>
@@ -1315,12 +1318,12 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="51">
+      <c r="A3" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="49">
         <f>$D$2*(SUM($E6:$E15)/($C$16*100))</f>
         <v>200</v>
       </c>
@@ -1332,24 +1335,24 @@
       <c r="J3" s="2"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="48" t="s">
+      <c r="B4" s="62"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="46" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="66" t="s">
+      <c r="H4" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="68"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="66"/>
     </row>
     <row r="5" spans="1:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -1361,40 +1364,40 @@
       <c r="C5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="26" t="s">
+      <c r="D5" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>16</v>
+      <c r="F5" s="69" t="s">
+        <v>15</v>
       </c>
       <c r="G5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="31"/>
+      <c r="H5" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="29"/>
       <c r="K5" s="24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="34">
+        <v>18</v>
+      </c>
+      <c r="B6" s="32">
         <v>2</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="33">
         <v>100</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="34">
         <v>30</v>
       </c>
       <c r="E6" s="11">
@@ -1417,17 +1420,17 @@
         <f>ROUNDUP($F6,0)*60</f>
         <v>12000</v>
       </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="49">
+      <c r="J6" s="30"/>
+      <c r="K6" s="47">
         <f>$H$16*K12</f>
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="11">
         <f t="shared" ref="E7:E15" si="2">$C7*$B7</f>
         <v>0</v>
@@ -1448,14 +1451,14 @@
         <f t="shared" ref="I7:I15" si="4">ROUNDUP($F7,0)*60</f>
         <v>0</v>
       </c>
-      <c r="J7" s="32"/>
+      <c r="J7" s="30"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1472,20 +1475,20 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="53" t="s">
-        <v>14</v>
+      <c r="J8" s="30"/>
+      <c r="K8" s="51" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1502,18 +1505,18 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J9" s="32"/>
-      <c r="K9" s="54"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="52"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="39"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1534,14 +1537,14 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J10" s="32"/>
-      <c r="K10" s="54"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="52"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1562,14 +1565,14 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="55"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="53"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1590,16 +1593,16 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J12" s="33"/>
-      <c r="K12" s="47">
+      <c r="J12" s="31"/>
+      <c r="K12" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="43"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1620,13 +1623,13 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J13" s="33"/>
+      <c r="J13" s="31"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="39"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1647,13 +1650,13 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J14" s="33"/>
+      <c r="J14" s="31"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="46"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1674,18 +1677,18 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J15" s="33"/>
+      <c r="J15" s="31"/>
     </row>
     <row r="16" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="30" t="str">
+      <c r="C16" s="28" t="str">
         <f>_xlfn.CONCAT(SUM(C6:C15)," %")</f>
         <v>100 %</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="52">
+      <c r="F16" s="50">
         <f>SUM(F6:F15)</f>
         <v>200</v>
       </c>
@@ -1700,7 +1703,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Performance testing Release 1.3.x v0.5
Signed-off-by: Deepesh Gurung <deepesh.gurung@technoforte.co.in>
</commit_message>
<xml_diff>
--- a/performance-test/packet-credential-processing/MOSIP_TPS_Thread_setting_calculator-packet_credential_processing.xlsx
+++ b/performance-test/packet-credential-processing/MOSIP_TPS_Thread_setting_calculator-packet_credential_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PerfScripts\Release\Platform1.3.x\performance-test\packet-credential-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72FE6F6-6565-4169-BEFF-2580A7E8E909}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2D180F-C691-4DC9-8F1B-4003742B89C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00F0FE37-4E08-4BBA-8E9E-0C9A5473C445}"/>
   </bookViews>
@@ -22,6 +22,114 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Deepesh Gurung</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{12A6E68C-AEA6-4864-B912-9F7742D2B41D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+These values are obtained from Performance test plan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{D052B09E-DCF5-40D0-AB38-068455D53461}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This is obtained from Jmeter results of previous tests.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{E13D392D-DB89-48E3-AC0D-B1B093E487C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Apply these values Jmeter as thread setting for each scenario
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{FCDFD1EE-38D0-440C-9004-6D7924913778}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+apply this value in Jmeter for "RampUp" variable under "user defined variables")
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -170,7 +278,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +394,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -888,6 +1009,15 @@
     <xf numFmtId="164" fontId="6" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -935,15 +1065,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1264,11 +1385,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EF0A02-FD69-493C-AB91-7265D86F2CBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EF0A02-FD69-493C-AB91-7265D86F2CBF}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,25 +1408,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="H1" s="58" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="H1" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="63"/>
       <c r="D2" s="48">
         <v>100</v>
       </c>
@@ -1318,11 +1439,11 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="49">
         <f>$D$2*(SUM($E6:$E15)/($C$16*100))</f>
         <v>200</v>
@@ -1336,23 +1457,23 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="46" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="66"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -1364,13 +1485,13 @@
       <c r="C5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="F5" s="53" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="23" t="s">
@@ -1480,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="30"/>
-      <c r="K8" s="51" t="s">
+      <c r="K8" s="54" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1510,7 +1631,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="30"/>
-      <c r="K9" s="52"/>
+      <c r="K9" s="55"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
@@ -1538,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="30"/>
-      <c r="K10" s="52"/>
+      <c r="K10" s="55"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
@@ -1566,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="30"/>
-      <c r="K11" s="53"/>
+      <c r="K11" s="56"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
@@ -1728,5 +1849,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>